<commit_message>
Updated Lessons Learned and documentation before github repo made public
</commit_message>
<xml_diff>
--- a/ArmServoAngularAccelCalcs.xlsx
+++ b/ArmServoAngularAccelCalcs.xlsx
@@ -1222,7 +1222,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1381,7 +1381,7 @@
         <v>70</v>
       </c>
       <c r="F6">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="G6">
         <v>45</v>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>1266.6666666666667</v>
+        <v>1150</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Updated to use gobilda servo for head Nod now,  use of New op
Updated to use gobilda servo for head Nod now instead of Hitec so that no longer have servo whine.  Also seems servo is as fast as the Hitec one so can run at 6V instead of 7.4 althouigh that is still an options if want faster operatoni.

Added -  use of New op with free to show can use New now.  Only use it for the LED device at the moment.
Also added in call to print freeMemory after New of LED device to see how much space use of New took up.
</commit_message>
<xml_diff>
--- a/ArmServoAngularAccelCalcs.xlsx
+++ b/ArmServoAngularAccelCalcs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\Halloween\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GregG\Documents\GitHub\Halloween\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28056" windowHeight="10992" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28050" windowHeight="10995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -159,6 +159,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Greg</author>
+    <author>Greg G</author>
   </authors>
   <commentList>
     <comment ref="I4" authorId="0" shapeId="0">
@@ -169,7 +170,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Greg:</t>
         </r>
@@ -178,10 +179,34 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 198 is chosen by setting resolution to normal instead of fine (fine makes it 120 degrees)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Greg G:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Degree setting sent to Servo device write method that will put servo position at its actual Center Point Pulse width. This allows all recording, etc to be reused as is, as the degree settings are translated to the correct pulse width to match a prior arbitrary servo position the user desires</t>
         </r>
       </text>
     </comment>
@@ -224,7 +249,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t>weight of object oz</t>
   </si>
@@ -415,13 +440,43 @@
   </si>
   <si>
     <t>Elbow Pitch</t>
+  </si>
+  <si>
+    <t>Center Point  pulse width</t>
+  </si>
+  <si>
+    <t>Center Point degrees</t>
+  </si>
+  <si>
+    <t>Remapped servo device  degree limited min</t>
+  </si>
+  <si>
+    <t>Remapped servo device  degree limited max</t>
+  </si>
+  <si>
+    <t>degree/pulse width</t>
+  </si>
+  <si>
+    <t>pulse width/degree</t>
+  </si>
+  <si>
+    <t>Remapped servo device  degree limited min calculated pulse width</t>
+  </si>
+  <si>
+    <t>Remapped servo device  degree limited max calculated pulse width</t>
+  </si>
+  <si>
+    <t>Remapped servo device degree want associated with actual servo Center Point degree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,19 +505,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -484,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -504,6 +546,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -790,15 +833,15 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -815,7 +858,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -832,7 +875,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -853,7 +896,7 @@
         <v>12.286948853615522</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -874,7 +917,7 @@
         <v>0.34864217372134043</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -891,7 +934,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -920,7 +963,7 @@
         <v>2.7129056798771294</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -941,7 +984,7 @@
         <v>252.55661375661373</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -962,7 +1005,7 @@
         <v>1.7834416188934554</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -983,7 +1026,7 @@
         <v>55.061628414881227</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1000,7 +1043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1017,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1038,7 +1081,7 @@
         <v>27.530814207440613</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1059,17 +1102,17 @@
         <v>1577.3994606451515</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1084,7 +1127,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1099,7 +1142,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -1112,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -1127,7 +1170,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -1142,7 +1185,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -1157,7 +1200,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
@@ -1169,7 +1212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>40</v>
       </c>
@@ -1181,7 +1224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -1193,16 +1236,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
@@ -1219,25 +1262,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.109375" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="61.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B1">
@@ -1268,8 +1311,8 @@
         <v>500</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B2">
@@ -1300,8 +1343,8 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3">
@@ -1332,8 +1375,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B4">
@@ -1364,279 +1407,462 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2">
+        <f>(K2+K1)/2</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2">
+        <f>(K4+K3)/2</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="9">
+        <f>(K4-K3)/(K2-K1)</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="9">
+        <f>1/K7</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6">
+      <c r="B10">
         <v>45</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
         <v>120</v>
       </c>
-      <c r="E6">
+      <c r="E10">
         <v>70</v>
       </c>
-      <c r="F6">
+      <c r="F10">
         <v>45</v>
       </c>
-      <c r="G6">
+      <c r="G10">
         <v>45</v>
       </c>
-      <c r="H6">
+      <c r="H10">
         <v>80</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7">
+      <c r="B11">
         <v>180</v>
       </c>
-      <c r="C7">
+      <c r="C11">
         <v>200</v>
       </c>
-      <c r="D7">
+      <c r="D11">
         <v>240</v>
       </c>
-      <c r="E7">
+      <c r="E11">
         <v>190</v>
       </c>
-      <c r="F7">
+      <c r="F11">
         <v>120</v>
       </c>
-      <c r="G7">
+      <c r="G11">
         <v>140</v>
       </c>
-      <c r="H7">
+      <c r="H11">
         <v>110</v>
       </c>
-      <c r="I7">
+      <c r="I11">
         <v>198</v>
       </c>
-      <c r="K7">
+      <c r="K11">
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2">
-        <f t="shared" ref="B8:H8" si="0">((B6-B3)*(B2-B1)/(B4-B3))+B1</f>
+      <c r="B12" s="2">
+        <f>((B10-B3)*(B2-B1)/(B4-B3))+B1</f>
         <v>800</v>
       </c>
-      <c r="C8" s="2">
-        <f t="shared" si="0"/>
+      <c r="C12" s="2">
+        <f>((C10-C3)*(C2-C1)/(C4-C3))+C1</f>
         <v>500</v>
       </c>
-      <c r="D8" s="2">
-        <f t="shared" si="0"/>
+      <c r="D12" s="2">
+        <f>((D10-D3)*(D2-D1)/(D4-D3))+D1</f>
         <v>1300</v>
       </c>
-      <c r="E8" s="2">
-        <f t="shared" si="0"/>
+      <c r="E12" s="2">
+        <f>((E10-E3)*(E2-E1)/(E4-E3))+E1</f>
         <v>966.66666666666674</v>
       </c>
-      <c r="F8" s="2">
-        <f t="shared" si="0"/>
+      <c r="F12" s="2">
+        <f>((F10-F3)*(F2-F1)/(F4-F3))+F1</f>
         <v>1150</v>
       </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
+      <c r="G12" s="2">
+        <f>((G10-G3)*(G2-G1)/(G4-G3))+G1</f>
         <v>1150</v>
       </c>
-      <c r="H8" s="2">
-        <f t="shared" si="0"/>
+      <c r="H12" s="2">
+        <f>((H10-H3)*(H2-H1)/(H4-H3))+H1</f>
         <v>1422.2222222222222</v>
       </c>
-      <c r="I8" s="2">
-        <f t="shared" ref="I8" si="1">((I6-I3)*(I2-I1)/(I4-I3))+I1</f>
+      <c r="I12" s="2">
+        <f>((I10-I3)*(I2-I1)/(I4-I3))+I1</f>
         <v>900</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2">
-        <f t="shared" ref="K8" si="2">((K6-K3)*(K2-K1)/(K4-K3))+K1</f>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2">
+        <f>((K10-K3)*(K2-K1)/(K4-K3))+K1</f>
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="2">
-        <f t="shared" ref="B9:H9" si="3">((B7-B3)*(B2-B1)/(B4-B3))+B1</f>
+      <c r="B13" s="2">
+        <f>((B11-B3)*(B2-B1)/(B4-B3))+B1</f>
         <v>1700</v>
       </c>
-      <c r="C9" s="2">
-        <f t="shared" si="3"/>
+      <c r="C13" s="2">
+        <f>((C11-C3)*(C2-C1)/(C4-C3))+C1</f>
         <v>1833.3333333333333</v>
       </c>
-      <c r="D9" s="2">
-        <f t="shared" si="3"/>
+      <c r="D13" s="2">
+        <f>((D11-D3)*(D2-D1)/(D4-D3))+D1</f>
         <v>2100</v>
       </c>
-      <c r="E9" s="2">
-        <f t="shared" si="3"/>
+      <c r="E13" s="2">
+        <f>((E11-E3)*(E2-E1)/(E4-E3))+E1</f>
         <v>1766.6666666666667</v>
       </c>
-      <c r="F9" s="2">
-        <f t="shared" si="3"/>
+      <c r="F13" s="2">
+        <f>((F11-F3)*(F2-F1)/(F4-F3))+F1</f>
         <v>1733.3333333333335</v>
       </c>
-      <c r="G9" s="2">
-        <f t="shared" si="3"/>
+      <c r="G13" s="2">
+        <f>((G11-G3)*(G2-G1)/(G4-G3))+G1</f>
         <v>1888.8888888888889</v>
       </c>
-      <c r="H9" s="2">
-        <f t="shared" si="3"/>
+      <c r="H13" s="2">
+        <f>((H11-H3)*(H2-H1)/(H4-H3))+H1</f>
         <v>1655.5555555555557</v>
       </c>
-      <c r="I9" s="2">
-        <f t="shared" ref="I9" si="4">((I7-I3)*(I2-I1)/(I4-I3))+I1</f>
+      <c r="I13" s="2">
+        <f>((I11-I3)*(I2-I1)/(I4-I3))+I1</f>
         <v>2100</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2">
-        <f t="shared" ref="K9" si="5">((K7-K3)*(K2-K1)/(K4-K3))+K1</f>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2">
+        <f>((K11-K3)*(K2-K1)/(K4-K3))+K1</f>
         <v>1700</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2">
+        <f>((K17-K16)*K8)+K5</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2">
+        <f>((K18-K16)*K8)+K5</f>
+        <v>1833.3333333333335</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C22" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D22" t="s">
         <v>27</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E22" t="s">
         <v>62</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F22" t="s">
         <v>28</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G22" t="s">
         <v>29</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H22" t="s">
         <v>30</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I22" t="s">
         <v>59</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12">
+      <c r="B23">
         <v>90</v>
       </c>
-      <c r="C12">
+      <c r="C23">
         <v>180</v>
       </c>
-      <c r="D12">
+      <c r="D23">
         <v>120</v>
       </c>
-      <c r="E12">
+      <c r="E23">
         <v>180</v>
       </c>
-      <c r="F12">
+      <c r="F23">
         <v>90</v>
       </c>
-      <c r="G12">
+      <c r="G23">
         <v>90</v>
       </c>
-      <c r="H12">
+      <c r="H23">
         <v>110</v>
       </c>
-      <c r="I12">
+      <c r="I23">
         <v>165</v>
       </c>
-      <c r="K12">
+      <c r="K23">
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13">
+      <c r="B24">
         <v>44</v>
       </c>
-      <c r="C13">
+      <c r="C24">
         <v>46</v>
       </c>
-      <c r="D13">
+      <c r="D24">
         <v>45</v>
       </c>
-      <c r="E13">
+      <c r="E24">
         <v>2</v>
       </c>
-      <c r="F13">
+      <c r="F24">
         <v>11</v>
       </c>
-      <c r="G13">
+      <c r="G24">
         <v>12</v>
       </c>
-      <c r="H13">
+      <c r="H24">
         <v>13</v>
       </c>
-      <c r="I13">
+      <c r="I24">
         <v>46</v>
       </c>
-      <c r="K13">
+      <c r="K24">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14">
+      <c r="B25">
         <v>11</v>
       </c>
-      <c r="C14">
+      <c r="C25">
         <v>9</v>
       </c>
-      <c r="D14">
+      <c r="D25">
         <v>10</v>
       </c>
-      <c r="E14">
+      <c r="E25">
         <v>4</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
         <v>1</v>
       </c>
-      <c r="H14">
+      <c r="H25">
         <v>2</v>
       </c>
-      <c r="I14">
+      <c r="I25">
         <v>9</v>
       </c>
-      <c r="K14">
+      <c r="K25">
         <v>9</v>
       </c>
     </row>
@@ -1655,18 +1881,18 @@
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>43</v>
       </c>
@@ -1695,7 +1921,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
@@ -1742,7 +1968,7 @@
       </c>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -1788,7 +2014,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="144" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>55</v>
       </c>
@@ -1828,7 +2054,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
@@ -1868,7 +2094,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>60</v>
       </c>
@@ -1908,7 +2134,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N11" s="4"/>
     </row>
   </sheetData>

</xml_diff>